<commit_message>
fixes and latest code
</commit_message>
<xml_diff>
--- a/TestData/StageData.xlsx
+++ b/TestData/StageData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>testCaseID</t>
   </si>
@@ -79,19 +79,16 @@
     <t>Client call</t>
   </si>
   <si>
-    <t>24 Karat (Raj Jewellers+GANPATRAJ GOLD)</t>
-  </si>
-  <si>
-    <t>Adarsh jain</t>
+    <t>Berd</t>
+  </si>
+  <si>
+    <t>Jack</t>
   </si>
   <si>
     <t>Medium</t>
   </si>
   <si>
     <t>Client meeting</t>
-  </si>
-  <si>
-    <t>Exit360</t>
   </si>
   <si>
     <t>Shane watson</t>
@@ -120,12 +117,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,7 +138,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <color rgb="FF202124"/>
       <name val="Consolas"/>
@@ -151,34 +147,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF202124"/>
-      <name val="Consolas"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -198,9 +166,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -208,15 +176,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -269,8 +236,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -283,9 +259,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -313,187 +303,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -507,11 +497,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -531,41 +527,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -590,6 +556,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -604,151 +579,166 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -758,8 +748,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1021,8 +1011,8 @@
   <sheetPr/>
   <dimension ref="A1:W1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -1110,7 +1100,7 @@
       <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>22</v>
       </c>
       <c r="E2" t="s">
@@ -1120,34 +1110,34 @@
         <v>24</v>
       </c>
       <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>26</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="K2">
         <v>7896321458</v>
       </c>
       <c r="L2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s">
         <v>29</v>
       </c>
-      <c r="M2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="6">
+      <c r="N2" s="4">
         <v>5000</v>
       </c>
       <c r="O2">
         <v>60</v>
       </c>
       <c r="P2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q2">
         <v>8527903362</v>
@@ -1156,7 +1146,7 @@
         <v>20</v>
       </c>
       <c r="S2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1"/>

</xml_diff>